<commit_message>
Update Control Calidad - DATAMUJERES-Violencia.xlsx
</commit_message>
<xml_diff>
--- a/Control Calidad - DATAMUJERES-Violencia.xlsx
+++ b/Control Calidad - DATAMUJERES-Violencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karen\Dropbox\DI Monitoreo II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D24B9E3-1853-45D3-B770-0F495AC9629D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8ED559-D631-40C6-AC85-60D92C54635D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{690ACAAD-F20B-42F0-9863-A1E9DF93E593}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{690ACAAD-F20B-42F0-9863-A1E9DF93E593}"/>
   </bookViews>
   <sheets>
     <sheet name="Agricultura" sheetId="2" r:id="rId1"/>
@@ -673,7 +673,7 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>49530</xdr:colOff>
+      <xdr:colOff>46355</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:from>
@@ -681,7 +681,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>535305</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>144146</xdr:rowOff>
+      <xdr:rowOff>140971</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -751,15 +751,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>48260</xdr:colOff>
+      <xdr:colOff>45085</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>65406</xdr:rowOff>
+      <xdr:rowOff>68581</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>772795</xdr:colOff>
+      <xdr:colOff>769620</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>125096</xdr:rowOff>
+      <xdr:rowOff>121921</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
       <mc:Choice Requires="sle15">
@@ -835,7 +835,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1248410</xdr:colOff>
+      <xdr:colOff>1245235</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
@@ -1310,7 +1310,7 @@
       <pane xSplit="2" ySplit="10" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomRight" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>